<commit_message>
projekt dziala, dodano pokoje do pliku excel
</commit_message>
<xml_diff>
--- a/hotel_data.xlsx
+++ b/hotel_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>Room Number</t>
   </si>
@@ -44,16 +44,22 @@
     <t>2024-11-17</t>
   </si>
   <si>
-    <t>Tom Cruise</t>
+    <t>no</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Alice Smith, Bob Smith</t>
+  </si>
+  <si>
+    <t>2024-11-16</t>
+  </si>
+  <si>
+    <t>Donald Trump</t>
   </si>
   <si>
     <t>2024-11-19</t>
-  </si>
-  <si>
-    <t>Alice Smith, Bob Smith</t>
-  </si>
-  <si>
-    <t>2024-11-16</t>
   </si>
 </sst>
 </file>
@@ -98,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -161,16 +167,16 @@
         <v>1.0</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="G3" t="n" s="0">
-        <v>3.0</v>
+      <c r="G3" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -194,6 +200,190 @@
       </c>
       <c r="G4" t="n" s="0">
         <v>5.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>104.0</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>105.0</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>201.0</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>200.0</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>202.0</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G8" t="n" s="0">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>203.0</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>300.0</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>204.0</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>205.0</v>
+      </c>
+      <c r="B11" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>301.0</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
projekt w formie zaliczeniowej
</commit_message>
<xml_diff>
--- a/hotel_data.xlsx
+++ b/hotel_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
   <si>
     <t>Room Number</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Elon Musk</t>
+  </si>
+  <si>
+    <t>2024-11-10</t>
   </si>
 </sst>
 </file>
@@ -383,10 +386,10 @@
         <v>16</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G12" t="n" s="0">
-        <v>3.0</v>
+        <v>20.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>